<commit_message>
fix: change new_data file
</commit_message>
<xml_diff>
--- a/ecowas/new_data.xlsx
+++ b/ecowas/new_data.xlsx
@@ -10,8 +10,8 @@
   </definedNames>
   <calcPr/>
   <extLst>
-    <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="Q2YlBMeAOYQ8zc5RzlXNt1GOXh/Q1b1WAbm2kdOsi2c="/>
+    <ext uri="GoogleSheetsCustomDataVersion1">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mjrElENqAKLTA0DIYNVzjqy9S2ukA=="/>
     </ext>
   </extLst>
 </workbook>
@@ -119,7 +119,7 @@
     <t>Guinea Bissau</t>
   </si>
   <si>
-    <t>Gambia, The</t>
+    <t>The Gambia</t>
   </si>
   <si>
     <t>Togo</t>
@@ -579,10 +579,10 @@
     <xf borderId="4" fillId="0" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -3355,7 +3355,7 @@
       </c>
     </row>
     <row r="54" ht="15.75" customHeight="1">
-      <c r="A54" s="6" t="s">
+      <c r="A54" s="14" t="s">
         <v>33</v>
       </c>
       <c r="B54" s="6" t="s">
@@ -3402,7 +3402,7 @@
       </c>
     </row>
     <row r="55" ht="15.75" customHeight="1">
-      <c r="A55" s="6" t="s">
+      <c r="A55" s="14" t="s">
         <v>33</v>
       </c>
       <c r="B55" s="6" t="s">
@@ -3449,7 +3449,7 @@
       </c>
     </row>
     <row r="56" ht="15.75" customHeight="1">
-      <c r="A56" s="6" t="s">
+      <c r="A56" s="14" t="s">
         <v>33</v>
       </c>
       <c r="B56" s="6" t="s">
@@ -3496,7 +3496,7 @@
       </c>
     </row>
     <row r="57" ht="15.75" customHeight="1">
-      <c r="A57" s="6" t="s">
+      <c r="A57" s="14" t="s">
         <v>33</v>
       </c>
       <c r="B57" s="6" t="s">
@@ -3727,10 +3727,10 @@
       </c>
     </row>
     <row r="62" ht="15.75" customHeight="1">
-      <c r="A62" s="14" t="s">
+      <c r="A62" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B62" s="15" t="s">
+      <c r="B62" s="14" t="s">
         <v>18</v>
       </c>
       <c r="C62" s="16" t="s">
@@ -3772,10 +3772,10 @@
       </c>
     </row>
     <row r="63" ht="15.75" customHeight="1">
-      <c r="A63" s="14" t="s">
+      <c r="A63" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B63" s="15" t="s">
+      <c r="B63" s="14" t="s">
         <v>36</v>
       </c>
       <c r="C63" s="16" t="s">
@@ -3817,10 +3817,10 @@
       </c>
     </row>
     <row r="64" ht="15.75" customHeight="1">
-      <c r="A64" s="14" t="s">
+      <c r="A64" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B64" s="15" t="s">
+      <c r="B64" s="14" t="s">
         <v>38</v>
       </c>
       <c r="C64" s="16" t="s">
@@ -3854,10 +3854,10 @@
       </c>
     </row>
     <row r="65" ht="15.75" customHeight="1">
-      <c r="A65" s="14" t="s">
+      <c r="A65" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B65" s="15" t="s">
+      <c r="B65" s="14" t="s">
         <v>40</v>
       </c>
       <c r="C65" s="16" t="s">
@@ -3899,10 +3899,10 @@
       </c>
     </row>
     <row r="66" ht="15.75" customHeight="1">
-      <c r="A66" s="14" t="s">
+      <c r="A66" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B66" s="15" t="s">
+      <c r="B66" s="14" t="s">
         <v>42</v>
       </c>
       <c r="C66" s="16" t="s">
@@ -3944,10 +3944,10 @@
       </c>
     </row>
     <row r="67" ht="15.75" customHeight="1">
-      <c r="A67" s="14" t="s">
+      <c r="A67" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B67" s="15" t="s">
+      <c r="B67" s="14" t="s">
         <v>44</v>
       </c>
       <c r="C67" s="16" t="s">
@@ -3989,10 +3989,10 @@
       </c>
     </row>
     <row r="68" ht="15.75" customHeight="1">
-      <c r="A68" s="14" t="s">
+      <c r="A68" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B68" s="15" t="s">
+      <c r="B68" s="14" t="s">
         <v>46</v>
       </c>
       <c r="C68" s="16" t="s">
@@ -4034,10 +4034,10 @@
       </c>
     </row>
     <row r="69" ht="15.75" customHeight="1">
-      <c r="A69" s="14" t="s">
+      <c r="A69" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B69" s="15" t="s">
+      <c r="B69" s="14" t="s">
         <v>48</v>
       </c>
       <c r="C69" s="16" t="s">
@@ -4079,10 +4079,10 @@
       </c>
     </row>
     <row r="70" ht="15.75" customHeight="1">
-      <c r="A70" s="14" t="s">
+      <c r="A70" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B70" s="15" t="s">
+      <c r="B70" s="14" t="s">
         <v>19</v>
       </c>
       <c r="C70" s="16" t="s">
@@ -4124,10 +4124,10 @@
       </c>
     </row>
     <row r="71" ht="15.75" customHeight="1">
-      <c r="A71" s="14" t="s">
+      <c r="A71" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B71" s="15" t="s">
+      <c r="B71" s="14" t="s">
         <v>50</v>
       </c>
       <c r="C71" s="16" t="s">
@@ -4169,10 +4169,10 @@
       </c>
     </row>
     <row r="72" ht="15.75" customHeight="1">
-      <c r="A72" s="14" t="s">
+      <c r="A72" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B72" s="15" t="s">
+      <c r="B72" s="14" t="s">
         <v>52</v>
       </c>
       <c r="C72" s="16" t="s">
@@ -4214,10 +4214,10 @@
       </c>
     </row>
     <row r="73" ht="15.75" customHeight="1">
-      <c r="A73" s="14" t="s">
+      <c r="A73" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B73" s="15" t="s">
+      <c r="B73" s="14" t="s">
         <v>54</v>
       </c>
       <c r="C73" s="16" t="s">
@@ -4259,10 +4259,10 @@
       </c>
     </row>
     <row r="74" ht="15.75" customHeight="1">
-      <c r="A74" s="14" t="s">
+      <c r="A74" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B74" s="15" t="s">
+      <c r="B74" s="14" t="s">
         <v>56</v>
       </c>
       <c r="C74" s="16" t="s">
@@ -4304,10 +4304,10 @@
       </c>
     </row>
     <row r="75" ht="15.75" customHeight="1">
-      <c r="A75" s="14" t="s">
+      <c r="A75" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B75" s="15" t="s">
+      <c r="B75" s="14" t="s">
         <v>57</v>
       </c>
       <c r="C75" s="16" t="s">
@@ -4349,10 +4349,10 @@
       </c>
     </row>
     <row r="76" ht="15.75" customHeight="1">
-      <c r="A76" s="14" t="s">
+      <c r="A76" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B76" s="15" t="s">
+      <c r="B76" s="14" t="s">
         <v>59</v>
       </c>
       <c r="C76" s="16" t="s">
@@ -4394,10 +4394,10 @@
       </c>
     </row>
     <row r="77" ht="15.75" customHeight="1">
-      <c r="A77" s="14" t="s">
+      <c r="A77" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B77" s="15" t="s">
+      <c r="B77" s="14" t="s">
         <v>61</v>
       </c>
       <c r="C77" s="16" t="s">
@@ -4439,10 +4439,10 @@
       </c>
     </row>
     <row r="78" ht="15.75" customHeight="1">
-      <c r="A78" s="14" t="s">
+      <c r="A78" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B78" s="15" t="s">
+      <c r="B78" s="14" t="s">
         <v>63</v>
       </c>
       <c r="C78" s="16" t="s">
@@ -4484,10 +4484,10 @@
       </c>
     </row>
     <row r="79" ht="15.75" customHeight="1">
-      <c r="A79" s="14" t="s">
+      <c r="A79" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B79" s="15" t="s">
+      <c r="B79" s="14" t="s">
         <v>20</v>
       </c>
       <c r="C79" s="16" t="s">
@@ -4529,10 +4529,10 @@
       </c>
     </row>
     <row r="80" ht="15.75" customHeight="1">
-      <c r="A80" s="14" t="s">
+      <c r="A80" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B80" s="15" t="s">
+      <c r="B80" s="14" t="s">
         <v>65</v>
       </c>
       <c r="C80" s="16" t="s">
@@ -4574,10 +4574,10 @@
       </c>
     </row>
     <row r="81" ht="15.75" customHeight="1">
-      <c r="A81" s="14" t="s">
+      <c r="A81" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B81" s="15" t="s">
+      <c r="B81" s="14" t="s">
         <v>67</v>
       </c>
       <c r="C81" s="16" t="s">
@@ -4619,10 +4619,10 @@
       </c>
     </row>
     <row r="82" ht="15.75" customHeight="1">
-      <c r="A82" s="14" t="s">
+      <c r="A82" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B82" s="15" t="s">
+      <c r="B82" s="14" t="s">
         <v>69</v>
       </c>
       <c r="C82" s="16" t="s">
@@ -4664,10 +4664,10 @@
       </c>
     </row>
     <row r="83" ht="15.75" customHeight="1">
-      <c r="A83" s="14" t="s">
+      <c r="A83" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B83" s="15" t="s">
+      <c r="B83" s="14" t="s">
         <v>16</v>
       </c>
       <c r="C83" s="16" t="s">
@@ -14861,7 +14861,7 @@
       </c>
     </row>
     <row r="300" ht="15.75" customHeight="1">
-      <c r="A300" s="26" t="s">
+      <c r="A300" s="15" t="s">
         <v>33</v>
       </c>
       <c r="B300" s="6" t="s">
@@ -14908,7 +14908,7 @@
       </c>
     </row>
     <row r="301" ht="15.75" customHeight="1">
-      <c r="A301" s="26" t="s">
+      <c r="A301" s="15" t="s">
         <v>33</v>
       </c>
       <c r="B301" s="6" t="s">
@@ -14955,7 +14955,7 @@
       </c>
     </row>
     <row r="302" ht="15.75" customHeight="1">
-      <c r="A302" s="26" t="s">
+      <c r="A302" s="15" t="s">
         <v>33</v>
       </c>
       <c r="B302" s="6" t="s">
@@ -15002,7 +15002,7 @@
       </c>
     </row>
     <row r="303" ht="15.75" customHeight="1">
-      <c r="A303" s="26" t="s">
+      <c r="A303" s="15" t="s">
         <v>33</v>
       </c>
       <c r="B303" s="6" t="s">
@@ -15049,7 +15049,7 @@
       </c>
     </row>
     <row r="304" ht="15.75" customHeight="1">
-      <c r="A304" s="26" t="s">
+      <c r="A304" s="15" t="s">
         <v>33</v>
       </c>
       <c r="B304" s="6" t="s">
@@ -15096,7 +15096,7 @@
       </c>
     </row>
     <row r="305" ht="15.75" customHeight="1">
-      <c r="A305" s="26" t="s">
+      <c r="A305" s="15" t="s">
         <v>33</v>
       </c>
       <c r="B305" s="6" t="s">
@@ -15143,7 +15143,7 @@
       </c>
     </row>
     <row r="306" ht="15.75" customHeight="1">
-      <c r="A306" s="26" t="s">
+      <c r="A306" s="15" t="s">
         <v>33</v>
       </c>
       <c r="B306" s="6" t="s">
@@ -15190,7 +15190,7 @@
       </c>
     </row>
     <row r="307" ht="15.75" customHeight="1">
-      <c r="A307" s="26" t="s">
+      <c r="A307" s="15" t="s">
         <v>33</v>
       </c>
       <c r="B307" s="6" t="s">
@@ -15237,7 +15237,7 @@
       </c>
     </row>
     <row r="308" ht="15.75" customHeight="1">
-      <c r="A308" s="26" t="s">
+      <c r="A308" s="15" t="s">
         <v>33</v>
       </c>
       <c r="B308" s="6" t="s">
@@ -15284,7 +15284,7 @@
       </c>
     </row>
     <row r="309" ht="15.75" customHeight="1">
-      <c r="A309" s="26" t="s">
+      <c r="A309" s="15" t="s">
         <v>33</v>
       </c>
       <c r="B309" s="6" t="s">
@@ -15331,7 +15331,7 @@
       </c>
     </row>
     <row r="310" ht="15.75" customHeight="1">
-      <c r="A310" s="26" t="s">
+      <c r="A310" s="15" t="s">
         <v>33</v>
       </c>
       <c r="B310" s="6" t="s">
@@ -15378,7 +15378,7 @@
       </c>
     </row>
     <row r="311" ht="15.75" customHeight="1">
-      <c r="A311" s="26" t="s">
+      <c r="A311" s="15" t="s">
         <v>33</v>
       </c>
       <c r="B311" s="6" t="s">
@@ -15425,7 +15425,7 @@
       </c>
     </row>
     <row r="312" ht="15.75" customHeight="1">
-      <c r="A312" s="26" t="s">
+      <c r="A312" s="15" t="s">
         <v>33</v>
       </c>
       <c r="B312" s="6" t="s">
@@ -15472,7 +15472,7 @@
       </c>
     </row>
     <row r="313" ht="15.75" customHeight="1">
-      <c r="A313" s="26" t="s">
+      <c r="A313" s="15" t="s">
         <v>33</v>
       </c>
       <c r="B313" s="6" t="s">
@@ -15519,7 +15519,7 @@
       </c>
     </row>
     <row r="314" ht="15.75" customHeight="1">
-      <c r="A314" s="26" t="s">
+      <c r="A314" s="15" t="s">
         <v>33</v>
       </c>
       <c r="B314" s="6" t="s">
@@ -15566,7 +15566,7 @@
       </c>
     </row>
     <row r="315" ht="15.75" customHeight="1">
-      <c r="A315" s="26" t="s">
+      <c r="A315" s="15" t="s">
         <v>33</v>
       </c>
       <c r="B315" s="6" t="s">
@@ -15613,7 +15613,7 @@
       </c>
     </row>
     <row r="316" ht="15.75" customHeight="1">
-      <c r="A316" s="26" t="s">
+      <c r="A316" s="15" t="s">
         <v>33</v>
       </c>
       <c r="B316" s="6" t="s">
@@ -15660,7 +15660,7 @@
       </c>
     </row>
     <row r="317" ht="15.75" customHeight="1">
-      <c r="A317" s="26" t="s">
+      <c r="A317" s="15" t="s">
         <v>33</v>
       </c>
       <c r="B317" s="6" t="s">
@@ -18335,7 +18335,7 @@
       </c>
     </row>
     <row r="406" ht="15.75" customHeight="1">
-      <c r="A406" s="6" t="s">
+      <c r="A406" s="14" t="s">
         <v>33</v>
       </c>
       <c r="B406" s="6" t="s">
@@ -18353,7 +18353,7 @@
       </c>
     </row>
     <row r="407" ht="15.75" customHeight="1">
-      <c r="A407" s="6" t="s">
+      <c r="A407" s="14" t="s">
         <v>33</v>
       </c>
       <c r="B407" s="6" t="s">
@@ -18371,7 +18371,7 @@
       </c>
     </row>
     <row r="408" ht="15.75" customHeight="1">
-      <c r="A408" s="6" t="s">
+      <c r="A408" s="14" t="s">
         <v>33</v>
       </c>
       <c r="B408" s="6" t="s">
@@ -18389,7 +18389,7 @@
       </c>
     </row>
     <row r="409" ht="15.75" customHeight="1">
-      <c r="A409" s="6" t="s">
+      <c r="A409" s="14" t="s">
         <v>33</v>
       </c>
       <c r="B409" s="6" t="s">
@@ -21027,7 +21027,7 @@
       </c>
     </row>
     <row r="575" ht="15.75" customHeight="1">
-      <c r="A575" s="26" t="s">
+      <c r="A575" s="15" t="s">
         <v>33</v>
       </c>
       <c r="B575" s="6" t="s">
@@ -21043,7 +21043,7 @@
       </c>
     </row>
     <row r="576" ht="15.75" customHeight="1">
-      <c r="A576" s="26" t="s">
+      <c r="A576" s="15" t="s">
         <v>33</v>
       </c>
       <c r="B576" s="6" t="s">
@@ -21059,7 +21059,7 @@
       </c>
     </row>
     <row r="577" ht="15.75" customHeight="1">
-      <c r="A577" s="26" t="s">
+      <c r="A577" s="15" t="s">
         <v>33</v>
       </c>
       <c r="B577" s="6" t="s">
@@ -21075,7 +21075,7 @@
       </c>
     </row>
     <row r="578" ht="15.75" customHeight="1">
-      <c r="A578" s="26" t="s">
+      <c r="A578" s="15" t="s">
         <v>33</v>
       </c>
       <c r="B578" s="6" t="s">
@@ -21091,7 +21091,7 @@
       </c>
     </row>
     <row r="579" ht="15.75" customHeight="1">
-      <c r="A579" s="26" t="s">
+      <c r="A579" s="15" t="s">
         <v>33</v>
       </c>
       <c r="B579" s="6" t="s">
@@ -21107,7 +21107,7 @@
       </c>
     </row>
     <row r="580" ht="15.75" customHeight="1">
-      <c r="A580" s="26" t="s">
+      <c r="A580" s="15" t="s">
         <v>33</v>
       </c>
       <c r="B580" s="6" t="s">
@@ -21123,7 +21123,7 @@
       </c>
     </row>
     <row r="581" ht="15.75" customHeight="1">
-      <c r="A581" s="26" t="s">
+      <c r="A581" s="15" t="s">
         <v>33</v>
       </c>
       <c r="B581" s="6" t="s">
@@ -21139,7 +21139,7 @@
       </c>
     </row>
     <row r="582" ht="15.75" customHeight="1">
-      <c r="A582" s="26" t="s">
+      <c r="A582" s="15" t="s">
         <v>33</v>
       </c>
       <c r="B582" s="6" t="s">
@@ -21155,7 +21155,7 @@
       </c>
     </row>
     <row r="583" ht="15.75" customHeight="1">
-      <c r="A583" s="26" t="s">
+      <c r="A583" s="15" t="s">
         <v>33</v>
       </c>
       <c r="B583" s="6" t="s">
@@ -21171,7 +21171,7 @@
       </c>
     </row>
     <row r="584" ht="15.75" customHeight="1">
-      <c r="A584" s="26" t="s">
+      <c r="A584" s="15" t="s">
         <v>33</v>
       </c>
       <c r="B584" s="6" t="s">
@@ -21185,7 +21185,7 @@
       </c>
     </row>
     <row r="585" ht="15.75" customHeight="1">
-      <c r="A585" s="26" t="s">
+      <c r="A585" s="15" t="s">
         <v>33</v>
       </c>
       <c r="B585" s="6" t="s">
@@ -21201,7 +21201,7 @@
       </c>
     </row>
     <row r="586" ht="15.75" customHeight="1">
-      <c r="A586" s="26" t="s">
+      <c r="A586" s="15" t="s">
         <v>33</v>
       </c>
       <c r="B586" s="6" t="s">

</xml_diff>